<commit_message>
Fix on data file caused bugs
</commit_message>
<xml_diff>
--- a/script/data/defaultrules.xlsx
+++ b/script/data/defaultrules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonogenesis-flask\script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87A35FA-546C-486D-BB9A-28350472275C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B623B427-DBF0-4CFC-9D9E-6349751A91DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
   </bookViews>
@@ -552,9 +552,6 @@
     <t>[velar,oral stop]&gt;[coronal,postalveolar,affricate,posterior,laminal,strident,(backness),(height)]/_[front,vowel]</t>
   </si>
   <si>
-    <t>[velar,oral stop]&gt;[coronal,postalveolar,fricative,posterior,laminal,strident,(backness),(height)]/_[front,vowel]</t>
-  </si>
-  <si>
     <t>[velar,oral stop]&gt;[coronal,alveolar,affricate,anterior,apical,strident,(backness),(height)]/_[front,vowel]</t>
   </si>
   <si>
@@ -601,6 +598,9 @@
   </si>
   <si>
     <t>[oral stop,voiced]&amp;[affricate,voiced]&gt;[voiceless]/_#</t>
+  </si>
+  <si>
+    <t>[velar,oral stop]&gt;[coronal,postalveolar,fricative,continuant,posterior,laminal,strident,(backness),(height)]/_[front,vowel]</t>
   </si>
 </sst>
 </file>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EDC81-2F31-2B49-AF42-0AADC8A78E53}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:XFD102"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B45" t="s">
         <v>133</v>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B48" t="s">
         <v>51</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B49" t="s">
         <v>147</v>
@@ -1969,10 +1969,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B106" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C106" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Fix on small issues, prepare big structural change
</commit_message>
<xml_diff>
--- a/script/data/defaultrules.xlsx
+++ b/script/data/defaultrules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonogenesis-flask\script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B623B427-DBF0-4CFC-9D9E-6349751A91DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5ECC8A-C161-4980-B348-9F83A162689F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
   </bookViews>
   <sheets>
     <sheet name="defaultrules" sheetId="1" r:id="rId1"/>
@@ -402,30 +402,18 @@
     <t>&lt;&lt;PREDEFINED&gt;&gt;{'s':'h'}/_#&amp;_[consonant][consonant]</t>
   </si>
   <si>
-    <t>[alveolar,oral stop]&gt;[fricative,strident]/_[front,vowel]</t>
-  </si>
-  <si>
     <t>[alveolar,oral stop]&gt;[affricate,strident]/_[front,vowel]</t>
   </si>
   <si>
     <t>[alveolar,oral stop]&gt;[postalveolar,affricate,posterior,laminal,strident]/_[front,vowel]</t>
   </si>
   <si>
-    <t>[alveolar,oral stop]&gt;[postalveolar,fricative,posterior,laminal,strident]/_[front,vowel]</t>
-  </si>
-  <si>
     <t>[alveolar,oral stop]&gt;[postalveolar,affricate,posterior,laminal,strident]/_[high,front,vowel]</t>
   </si>
   <si>
-    <t>[alveolar,oral stop]&gt;[postalveolar,fricative,posterior,laminal,strident]/_[high,front,vowel]</t>
-  </si>
-  <si>
     <t>[alveolar,oral stop]&gt;[affricate,strident]/_[high,front,vowel]</t>
   </si>
   <si>
-    <t>[alveolar,oral stop]&gt;[fricative,strident]/_[high,front,vowel]</t>
-  </si>
-  <si>
     <t>palatalization of velar fricatives before front vowels</t>
   </si>
   <si>
@@ -555,21 +543,12 @@
     <t>[velar,oral stop]&gt;[coronal,alveolar,affricate,anterior,apical,strident,(backness),(height)]/_[front,vowel]</t>
   </si>
   <si>
-    <t>[velar,oral stop]&gt;[coronal,alveolar,fricative,anterior,apical,strident,(backness),(height)]/_[front,vowel]</t>
-  </si>
-  <si>
     <t>[velar,oral stop]&gt;[coronal,postalveolar,affricate,posterior,laminal,strident,(backness),(height)]/_[high,front,vowel]</t>
   </si>
   <si>
-    <t>[velar,oral stop]&gt;[coronal,postalveolar,fricative,posterior,laminal,strident,(backness),(height)]/_[high,front,vowel]</t>
-  </si>
-  <si>
     <t>[velar,oral stop]&gt;[coronal,alveolar,affricate,anterior,apical,strident,(backness),(height)]/_[high,front,vowel]</t>
   </si>
   <si>
-    <t>[velar,oral stop]&gt;[coronal,alveolar,fricative,anterior,apical,strident,(backness),(height)]/_[high,front,vowel]</t>
-  </si>
-  <si>
     <t>[velar,consonant]&gt;[palatal,front,posterior,laminal,(secondary POA),(stridency)]/[front,vowel]_</t>
   </si>
   <si>
@@ -601,6 +580,27 @@
   </si>
   <si>
     <t>[velar,oral stop]&gt;[coronal,postalveolar,fricative,continuant,posterior,laminal,strident,(backness),(height)]/_[front,vowel]</t>
+  </si>
+  <si>
+    <t>[velar,oral stop]&gt;[coronal,postalveolar,fricative,continuant,posterior,laminal,strident,(backness),(height)]/_[high,front,vowel]</t>
+  </si>
+  <si>
+    <t>[velar,oral stop]&gt;[coronal,alveolar,fricative,continuant,anterior,apical,strident,(backness),(height)]/_[front,vowel]</t>
+  </si>
+  <si>
+    <t>[alveolar,oral stop]&gt;[postalveolar,fricative,continuant,posterior,laminal,strident]/_[front,vowel]</t>
+  </si>
+  <si>
+    <t>[alveolar,oral stop]&gt;[fricative,continuant,strident]/_[front,vowel]</t>
+  </si>
+  <si>
+    <t>[velar,oral stop]&gt;[coronal,alveolar,fricative,continuant,anterior,apical,strident,(backness),(height)]/_[high,front,vowel]</t>
+  </si>
+  <si>
+    <t>[alveolar,oral stop]&gt;[postalveolar,fricative,continuant,posterior,laminal,strident]/_[high,front,vowel]</t>
+  </si>
+  <si>
+    <t>[alveolar,oral stop]&gt;[fricative,continuant,strident]/_[high,front,vowel]</t>
   </si>
 </sst>
 </file>
@@ -955,18 +955,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EDC81-2F31-2B49-AF42-0AADC8A78E53}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97.125" customWidth="1"/>
     <col min="2" max="2" width="72.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -977,9 +977,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -988,9 +988,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -999,9 +999,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1010,9 +1010,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1021,7 +1021,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1032,9 +1032,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1043,9 +1043,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1054,9 +1054,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -1065,9 +1065,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1076,9 +1076,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1087,9 +1087,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -1098,9 +1098,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -1109,9 +1109,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1120,9 +1120,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
@@ -1131,7 +1131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>113</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>114</v>
       </c>
@@ -1164,9 +1164,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B23" t="s">
         <v>92</v>
@@ -1175,9 +1175,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B24" t="s">
         <v>93</v>
@@ -1186,9 +1186,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1197,9 +1197,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1208,9 +1208,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -1219,9 +1219,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -1230,9 +1230,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
@@ -1241,9 +1241,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>187</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -1252,9 +1252,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
@@ -1263,9 +1263,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
@@ -1274,9 +1274,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
@@ -1285,9 +1285,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -1296,9 +1296,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
@@ -1307,9 +1307,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
@@ -1318,9 +1318,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -1329,9 +1329,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
@@ -1340,9 +1340,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
@@ -1351,9 +1351,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
@@ -1362,9 +1362,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
@@ -1373,9 +1373,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
@@ -1384,9 +1384,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -1395,20 +1395,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -1417,9 +1417,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
@@ -1428,9 +1428,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B48" t="s">
         <v>51</v>
@@ -1439,20 +1439,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1461,9 +1461,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
@@ -1472,9 +1472,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
         <v>26</v>
@@ -1483,9 +1483,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -1494,9 +1494,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B56" t="s">
         <v>14</v>
@@ -1505,9 +1505,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
@@ -1516,9 +1516,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
         <v>16</v>
@@ -1527,9 +1527,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
         <v>17</v>
@@ -1538,9 +1538,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
         <v>18</v>
@@ -1549,9 +1549,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
@@ -1560,9 +1560,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
         <v>53</v>
@@ -1571,9 +1571,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -1582,9 +1582,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
         <v>56</v>
@@ -1593,9 +1593,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
         <v>57</v>
@@ -1604,9 +1604,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
         <v>58</v>
@@ -1615,9 +1615,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
         <v>59</v>
@@ -1626,9 +1626,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B70" t="s">
         <v>60</v>
@@ -1637,9 +1637,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B71" t="s">
         <v>61</v>
@@ -1648,9 +1648,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
         <v>62</v>
@@ -1659,9 +1659,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
         <v>63</v>
@@ -1670,9 +1670,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
         <v>64</v>
@@ -1681,9 +1681,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
         <v>65</v>
@@ -1692,9 +1692,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B76" t="s">
         <v>66</v>
@@ -1703,9 +1703,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
         <v>67</v>
@@ -1714,9 +1714,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
         <v>68</v>
@@ -1725,9 +1725,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B79" t="s">
         <v>69</v>
@@ -1736,7 +1736,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>71</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>120</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>121</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>122</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>106</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>111</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>74</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>124</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>123</v>
       </c>
@@ -1967,12 +1967,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B106" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C106" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Partial Instructore mode. Modified hint and some small bugs.
</commit_message>
<xml_diff>
--- a/script/data/defaultrules.xlsx
+++ b/script/data/defaultrules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\accel\ProjectHome\phonogenesis-flask\script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5ECC8A-C161-4980-B348-9F83A162689F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F9FE66-7F96-487F-ACD1-09917E56C7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{C8F3CD5B-922F-8741-82D2-47D9CBF2A239}"/>
   </bookViews>
   <sheets>
     <sheet name="defaultrules" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="163">
   <si>
     <t>&lt;&lt;PREDEFINED&gt;&gt;{'k':'t͡ʃ','g':'d͡ʒ'}/_[front,vowel]</t>
   </si>
@@ -192,51 +192,6 @@
     <t>postnasal voicing of fricatives</t>
   </si>
   <si>
-    <t>voicing assimilation</t>
-  </si>
-  <si>
-    <t>regressive voicelessness assimilation in stops</t>
-  </si>
-  <si>
-    <t>regressive voicelessness assimilation in obstruents</t>
-  </si>
-  <si>
-    <t>regressive voicing assimilation in stops</t>
-  </si>
-  <si>
-    <t>regressive voicing assimilation in obstruents</t>
-  </si>
-  <si>
-    <t>regressive obstruent voicing assimilation in stops</t>
-  </si>
-  <si>
-    <t>regressive obstruent voicing assimilation in obstruents</t>
-  </si>
-  <si>
-    <t>progressive voicelessness assimilation in stops</t>
-  </si>
-  <si>
-    <t>progressive voicelessness assimilation in obstruents</t>
-  </si>
-  <si>
-    <t>progressive voicing assimilation in stops</t>
-  </si>
-  <si>
-    <t>progressive voicing assimilation in obstruents</t>
-  </si>
-  <si>
-    <t>progressive obstruent voicing assimilation in stops</t>
-  </si>
-  <si>
-    <t>progressive obstruent voicing assimilation in obstruents</t>
-  </si>
-  <si>
-    <t>voicelessness agreement between obstruents</t>
-  </si>
-  <si>
-    <t>voicing agreement between obstruents</t>
-  </si>
-  <si>
     <t>weird</t>
   </si>
   <si>
@@ -493,48 +448,6 @@
   </si>
   <si>
     <t>[fricative,voiceless]&gt;[voiced]/[nasal,consonant]_</t>
-  </si>
-  <si>
-    <t>[oral stop,voiced]&gt;[voiceless]/_[voiceless]</t>
-  </si>
-  <si>
-    <t>[obstruent,voiced]&gt;[voiceless]/_[voiceless]</t>
-  </si>
-  <si>
-    <t>[oral stop,voiceless]&gt;[voiced]/_[voiced,consonant]</t>
-  </si>
-  <si>
-    <t>[obstruent,voiceless]&gt;[voiced]/_[voiced,consonant]</t>
-  </si>
-  <si>
-    <t>[oral stop,voiceless]&gt;[voiced]/_[voiced,obstruent]</t>
-  </si>
-  <si>
-    <t>[obstruent,voiceless]&gt;[voiced]/_[voiced,obstruent]</t>
-  </si>
-  <si>
-    <t>[oral stop,voiced]&gt;[voiceless]/[voiceless]_</t>
-  </si>
-  <si>
-    <t>[obstruent,voiced]&gt;[voiceless]/[voiceless]_</t>
-  </si>
-  <si>
-    <t>[oral stop,voiceless]&gt;[voiced]/[voiced,consonant]_</t>
-  </si>
-  <si>
-    <t>[obstruent,voiceless]&gt;[voiced]/[voiced,consonant]_</t>
-  </si>
-  <si>
-    <t>[oral stop,voiceless]&gt;[voiced]/[voiced,obstruent]_</t>
-  </si>
-  <si>
-    <t>[obstruent,voiceless]&gt;[voiced]/[voiced,obstruent]_</t>
-  </si>
-  <si>
-    <t>[obstruent,voiceless]&gt;[voiced]/[voiceless,obstruent]_&amp;_[voiceless,obstruent]</t>
-  </si>
-  <si>
-    <t>[obstruent,voiceless]&gt;[voiced]/[voiced,obstruent]_&amp;_[voiced,obstruent]</t>
   </si>
   <si>
     <t>[velar,oral stop]&gt;[coronal,postalveolar,affricate,posterior,laminal,strident,(backness),(height)]/_[front,vowel]</t>
@@ -953,33 +866,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EDC81-2F31-2B49-AF42-0AADC8A78E53}">
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="97.125" customWidth="1"/>
     <col min="2" max="2" width="72.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -988,9 +901,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -999,9 +912,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1010,18 +923,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1032,9 +945,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1043,9 +956,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1054,9 +967,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -1065,9 +978,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1076,9 +989,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1087,9 +1000,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -1098,9 +1011,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -1109,9 +1022,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1120,9 +1033,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
@@ -1131,9 +1044,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
@@ -1142,9 +1055,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
@@ -1153,42 +1066,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>141</v>
-      </c>
-      <c r="B23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>170</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1197,9 +1110,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1208,9 +1121,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -1219,9 +1132,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -1230,9 +1143,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
@@ -1241,9 +1154,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -1252,9 +1165,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
@@ -1263,9 +1176,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
@@ -1274,9 +1187,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
@@ -1285,9 +1198,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -1296,9 +1209,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
@@ -1307,9 +1220,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
@@ -1318,9 +1231,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -1329,9 +1242,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
@@ -1340,9 +1253,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
@@ -1351,9 +1264,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
@@ -1362,9 +1275,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
@@ -1373,9 +1286,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
@@ -1384,9 +1297,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -1395,20 +1308,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -1417,9 +1330,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
@@ -1428,9 +1341,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
         <v>51</v>
@@ -1439,20 +1352,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1461,9 +1374,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
@@ -1472,9 +1385,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B53" t="s">
         <v>26</v>
@@ -1483,9 +1396,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -1494,9 +1407,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
         <v>14</v>
@@ -1505,9 +1418,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
@@ -1516,9 +1429,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
         <v>16</v>
@@ -1527,9 +1440,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s">
         <v>17</v>
@@ -1538,9 +1451,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
         <v>18</v>
@@ -1549,9 +1462,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
@@ -1560,9 +1473,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B63" t="s">
         <v>53</v>
@@ -1571,9 +1484,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -1582,183 +1495,183 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>156</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" t="s">
         <v>57</v>
       </c>
-      <c r="C67" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>160</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>162</v>
-      </c>
-      <c r="B72" t="s">
-        <v>62</v>
-      </c>
-      <c r="C72" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>163</v>
+        <v>65</v>
       </c>
       <c r="B73" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>167</v>
+        <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C78" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A80" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C81" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C82" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -1766,215 +1679,61 @@
         <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>97</v>
-      </c>
-      <c r="B84" t="s">
         <v>94</v>
       </c>
-      <c r="C84" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C89" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" t="s">
-        <v>84</v>
-      </c>
-      <c r="C90" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>86</v>
-      </c>
-      <c r="B92" t="s">
-        <v>87</v>
-      </c>
-      <c r="C92" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>112</v>
-      </c>
-      <c r="B93" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>121</v>
-      </c>
-      <c r="B94" t="s">
-        <v>89</v>
-      </c>
-      <c r="C94" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>122</v>
-      </c>
-      <c r="B95" t="s">
-        <v>90</v>
-      </c>
-      <c r="C95" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>106</v>
-      </c>
-      <c r="B96" t="s">
-        <v>105</v>
-      </c>
-      <c r="C96" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>108</v>
-      </c>
-      <c r="B97" t="s">
-        <v>107</v>
-      </c>
-      <c r="C97" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>111</v>
-      </c>
-      <c r="B98" t="s">
-        <v>110</v>
-      </c>
-      <c r="C98" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>74</v>
-      </c>
-      <c r="B100" t="s">
-        <v>102</v>
-      </c>
-      <c r="C100" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>104</v>
-      </c>
-      <c r="B101" t="s">
-        <v>103</v>
-      </c>
-      <c r="C101" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>124</v>
-      </c>
-      <c r="B103" t="s">
-        <v>75</v>
-      </c>
-      <c r="C103" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>123</v>
-      </c>
-      <c r="B104" t="s">
-        <v>78</v>
-      </c>
-      <c r="C104" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>183</v>
-      </c>
-      <c r="B106" t="s">
-        <v>182</v>
-      </c>
-      <c r="C106" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>